<commit_message>
updating Yrly numbers etc.
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,15 +146,6 @@
     <t>data.nba.net /prod/v1/20190125/scoreboard.json</t>
   </si>
   <si>
-    <t>data.nba.net /prod/v2/{{gameDate}}/scoreboard.json</t>
-  </si>
-  <si>
-    <t>data.nba.net /prod/v2/2018/teams.json</t>
-  </si>
-  <si>
-    <t>data.nba.net /prod/v1/2018/players.json</t>
-  </si>
-  <si>
     <t>data.nba.net /prod/v1/allstar/2018/AS_roster.json</t>
   </si>
   <si>
@@ -182,18 +173,6 @@
     <t>data.nba.net /prod/v1/2018/team_stats_last_five_games.json</t>
   </si>
   <si>
-    <t>data.nba.net /prod/v1/{{gameDate}}/{{gameId}}_preview_article.json</t>
-  </si>
-  <si>
-    <t>data.nba.net /prod/v1/{{gameDate}}/{{gameId}}_recap_article.json</t>
-  </si>
-  <si>
-    <t>data.nba.net /prod/v1/{{gameDate}}/{{gameId}}_Book.pdf</t>
-  </si>
-  <si>
-    <t>data.nba.net /prod/v1/{{gameDate}}/{{gameId}}_boxscore.json</t>
-  </si>
-  <si>
     <t>data.nba.net /prod/v1/{{gameDate}}/{{gameId}}_mini_boxscore.json</t>
   </si>
   <si>
@@ -206,9 +185,6 @@
     <t>data.nba.net /prod/v1/2018/players/{{personId}}_gamelog.json</t>
   </si>
   <si>
-    <t>data.nba.net /prod/v1/2018/players/{{personId}}_profile.json</t>
-  </si>
-  <si>
     <t>data.nba.net /prod/v1/2018/players/{{personId}}_uber_stats.json</t>
   </si>
   <si>
@@ -240,6 +216,30 @@
   </si>
   <si>
     <t>data.nba.net /prod/v1/2018/playoffs_{{seriesId}}_leaders.json</t>
+  </si>
+  <si>
+    <t>data.nba.net/prod/v2/{{gameDate}}/scoreboard.json</t>
+  </si>
+  <si>
+    <t>data.nba.net/prod/v1/{{gameDate}}/{{gameId}}_preview_article.json</t>
+  </si>
+  <si>
+    <t>data.nba.net/prod/v1/{{gameDate}}/{{gameId}}_recap_article.json</t>
+  </si>
+  <si>
+    <t>data.nba.net/prod/v1/{{gameDate}}/{{gameId}}_Book.pdf</t>
+  </si>
+  <si>
+    <t>data.nba.net/prod/v1/{{gameDate}}/{{gameId}}_boxscore.json</t>
+  </si>
+  <si>
+    <t>data.nba.net/prod/v1/2018/players/{{personId}}_profile.json</t>
+  </si>
+  <si>
+    <t>data.nba.net/prod/v2/2018/teams.json</t>
+  </si>
+  <si>
+    <t>data.nba.net/prod/v1/2018/players.json</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A2:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B6:B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +614,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -710,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -758,7 +758,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +798,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -806,7 +806,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,7 +814,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -830,7 +830,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload sql lite and other python files
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -246,13 +246,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -275,8 +281,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B38"/>
+  <dimension ref="A2:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D3" sqref="D3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +576,7 @@
     <col min="2" max="2" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -577,7 +584,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -585,15 +592,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -601,7 +609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -609,7 +617,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -617,7 +625,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -625,7 +633,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -633,7 +641,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -641,7 +649,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -649,7 +657,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -657,7 +665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -665,7 +673,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -673,7 +681,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -681,7 +689,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -867,5 +875,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>